<commit_message>
use extrapolation with scipy interp
</commit_message>
<xml_diff>
--- a/tests/test_v2.xlsx
+++ b/tests/test_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/python/excel-modelling-tools/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83099FC2-650A-F548-B94A-0855B9D15C71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA673E6-0F42-6E4D-B09B-83822AADFECB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1880" yWindow="3560" windowWidth="28560" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -629,7 +629,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
variability of uncertainty function is now relative to initial value of mean
</commit_message>
<xml_diff>
--- a/tests/test_v2.xlsx
+++ b/tests/test_v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/python/excel-modelling-tools/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA673E6-0F42-6E4D-B09B-83822AADFECB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6F8BF9-E789-3342-AFD2-E37CACBC787C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1880" yWindow="3560" windowWidth="28560" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -152,9 +152,6 @@
     <t>version</t>
   </si>
   <si>
-    <t>variability</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t>{"2010-01-01":1, "2010-03-01":100 , "2010-12-01":110}</t>
+  </si>
+  <si>
+    <t>initial_value_proportional_variation</t>
   </si>
 </sst>
 </file>
@@ -629,7 +629,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -648,25 +648,25 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>11</v>
@@ -686,13 +686,14 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <f>1/2.5</f>
+        <v>0.4</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>18</v>
@@ -715,16 +716,17 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" t="s">
-        <v>47</v>
-      </c>
       <c r="F3">
-        <v>4</v>
+        <f>1/2.5</f>
+        <v>0.4</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>18</v>

</xml_diff>